<commit_message>
WIP: local changes before sync with origin/main
</commit_message>
<xml_diff>
--- a/env-matrix.xlsx
+++ b/env-matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\ΑΠΟΔΕΙΞΗ ΚΑΙ ΒΕΒΑΙΩΣΗ ΙΑΝΟΥΑΡΙΟΥ-ΦΕΒΡΟΥΑΡΙΟΥ\CRYPTO\TELEGRAM APP\crypto-alerts-bot-paypal-eur FINAL\FINAL\crypto-alerts-plus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Desktop\ΑΠΟΔΕΙΞΗ ΚΑΙ ΒΕΒΑΙΩΣΗ ΙΑΝΟΥΑΡΙΟΥ-ΦΕΒΡΟΥΑΡΙΟΥ\CRYPTO\TELEGRAM APP\crypto-alerts-bot-paypal-eur FINAL\FINAL\clone\crypto-alerts-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F01922-499D-4284-9331-D7FA9D5C867D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC493619-F33E-49EB-9AAF-F69BAAAE2CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2028" yWindow="3372" windowWidth="19128" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4332" yWindow="2352" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single-service (recommended)" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>Service (example)</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>8290365345:AAGUwy0cFbSt3FLI2AmOjzaF21gvqJvw5Jc</t>
+  </si>
+  <si>
+    <t>8290365345:AAE9acNcVotxPc9JmbPxiueqC2NU64dO8ec</t>
   </si>
 </sst>
 </file>
@@ -202,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +215,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,13 +259,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -748,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,8 +1008,13 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="G8" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>